<commit_message>
base model done; cleaning nulls
</commit_message>
<xml_diff>
--- a/SQL_load/Schema_mapping.xlsx
+++ b/SQL_load/Schema_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulchung/Dropbox (Personal)/Paul Working Folder/Home/Coding/Metis/github_backup/Project-3-Classifier/SQL_load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648CB014-14CE-7040-922D-D0C4BAE5335B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA868A7C-3119-E444-AD45-672D31DDC236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33760" yWindow="1000" windowWidth="33760" windowHeight="19780" xr2:uid="{F0AF9B66-16F7-CB43-B2D9-075D61D3DF08}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="182">
   <si>
     <t>&lt;class 'pandas.core.frame.DataFrame'&gt;</t>
   </si>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7572D8-237D-FA4B-9AD9-423B3C5C3266}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,6 +1565,9 @@
       <c r="K34" t="s">
         <v>102</v>
       </c>
+      <c r="L34" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="N34" s="4"/>
       <c r="O34" t="s">
         <v>153</v>
@@ -1576,6 +1579,9 @@
       </c>
       <c r="K35" t="s">
         <v>103</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>159</v>

</xml_diff>